<commit_message>
refactored hack_angel n added official api for angel - working
</commit_message>
<xml_diff>
--- a/research/stock_returns_1yr.xlsx
+++ b/research/stock_returns_1yr.xlsx
@@ -490,20 +490,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ADANITRANS</t>
+          <t>ADANIENT</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1915.25</v>
+        <v>3841.2</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2549.5</v>
+        <v>44928</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -511,10 +513,12 @@
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I2" t="n">
-        <v>33.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -528,20 +532,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DEEPAKNTR</t>
+          <t>ADANITRANS</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2490.2</v>
+        <v>2549.5</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1989.15</v>
+        <v>44928</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -549,10 +555,12 @@
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-20.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -566,20 +574,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ADANIENT</t>
+          <t>DEEPAKNTR</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1709.45</v>
+        <v>1989.15</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3841.2</v>
+        <v>44928</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -587,10 +597,12 @@
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I4" t="n">
-        <v>124.7</v>
+        <v>45658</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -608,16 +620,18 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5890.35</v>
+        <v>3951.2</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3951.2</v>
+        <v>44928</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -625,10 +639,12 @@
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-32.9</v>
+        <v>45658</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -642,20 +658,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ALKYLAMINE</t>
+          <t>PERSISTENT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3547.7</v>
+        <v>4027.95</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2661.7</v>
+        <v>44928</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -663,10 +681,12 @@
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-25</v>
+        <v>45658</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -680,20 +700,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ESCORTS</t>
+          <t>ALKYLAMINE</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1908.7</v>
+        <v>2661.7</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2140.6</v>
+        <v>44928</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -701,10 +723,12 @@
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I7" t="n">
-        <v>12.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -718,20 +742,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NAUKRI</t>
+          <t>BAJFINANCE</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5576.7</v>
+        <v>6553.75</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3911.5</v>
+        <v>44928</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -739,10 +765,12 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-29.9</v>
+        <v>45658</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -756,20 +784,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BAJAJFINSV</t>
+          <t>LTIM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16406.2</v>
+        <v>4322.1</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1552.5</v>
+        <v>44928</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -777,10 +807,12 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-90.5</v>
+        <v>45658</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -794,20 +826,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MUTHOOTFIN</t>
+          <t>TITAN</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1495.65</v>
+        <v>2565.75</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1091.7</v>
+        <v>44928</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -815,10 +849,12 @@
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-27</v>
+        <v>45658</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -832,20 +868,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JKCEMENT</t>
+          <t>ATUL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3398.85</v>
+        <v>8207.6</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2955.95</v>
+        <v>44928</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -853,10 +891,12 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-13</v>
+        <v>45658</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -870,20 +910,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ATUL</t>
+          <t>NAUKRI</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9039.1</v>
+        <v>3911.5</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E12" t="n">
-        <v>8207.6</v>
+        <v>44928</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -891,10 +933,12 @@
         </is>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I12" t="n">
-        <v>-9.199999999999999</v>
+        <v>45658</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -908,20 +952,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>VINATIORGA</t>
+          <t>ESCORTS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1988.1</v>
+        <v>2140.6</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E13" t="n">
-        <v>2001.1</v>
+        <v>44928</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F13" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -929,10 +975,12 @@
         </is>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.7</v>
+        <v>45658</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -946,20 +994,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SUNDRMFAST</t>
+          <t>JKCEMENT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>912.8</v>
+        <v>2955.95</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E14" t="n">
-        <v>970</v>
+        <v>44928</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F14" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -967,10 +1017,12 @@
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I14" t="n">
-        <v>6.3</v>
+        <v>45658</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -984,20 +1036,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PAGEIND</t>
+          <t>MUTHOOTFIN</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>40421.55</v>
+        <v>1091.7</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E15" t="n">
-        <v>41921.05</v>
+        <v>44928</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F15" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1005,10 +1059,12 @@
         </is>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3.7</v>
+        <v>45658</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1022,20 +1078,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WHIRLPOOL</t>
+          <t>VINATIORGA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1761.75</v>
+        <v>2001.1</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1496.05</v>
+        <v>44928</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F16" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1043,10 +1101,12 @@
         </is>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I16" t="n">
-        <v>-15.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1060,20 +1120,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SHREECEM</t>
+          <t>SUNDRMFAST</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>26987.45</v>
+        <v>970</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E17" t="n">
-        <v>23454.7</v>
+        <v>44928</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F17" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1081,10 +1143,12 @@
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I17" t="n">
-        <v>-13.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1098,20 +1162,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LTIM</t>
+          <t>TIINDIA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7332</v>
+        <v>2785.3</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4322.1</v>
+        <v>44928</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F18" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1119,10 +1185,12 @@
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I18" t="n">
-        <v>-41.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1136,20 +1204,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BAJFINANCE</t>
+          <t>LINDEINDIA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6977.3</v>
+        <v>3540.45</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6553.75</v>
+        <v>44928</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F19" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1157,10 +1227,12 @@
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-6.1</v>
+        <v>45658</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1174,20 +1246,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PERSISTENT</t>
+          <t>TATAELXSI</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4904.35</v>
+        <v>6300.4</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4027.95</v>
+        <v>44928</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F20" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1195,10 +1269,12 @@
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I20" t="n">
-        <v>-17.9</v>
+        <v>45658</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1212,20 +1288,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TITAN</t>
+          <t>NAVINFLUOR</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2522.4</v>
+        <v>4122.4</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>44561</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2565.75</v>
+        <v>44928</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No Data</t>
+        </is>
       </c>
       <c r="F21" s="2" t="n">
-        <v>44926</v>
+        <v>45293</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1233,10 +1311,12 @@
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45291</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1.7</v>
+        <v>45658</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>

</xml_diff>